<commit_message>
KT ensuring all added
</commit_message>
<xml_diff>
--- a/MilkSheet/milk.xlsx
+++ b/MilkSheet/milk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.thompson/Projects/CoffeeCO-OP/MilkSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC71BC9C-0F08-A042-91C1-9A7B90E98C3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A2BB86-EF77-0C47-AEFA-E78BF37B587F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23740" windowHeight="19900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,15 +584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
@@ -626,136 +626,160 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19"/>
-    </row>
-    <row r="20" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="18" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="25" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
+    <row r="26" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="19"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="0.25" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="3"/>
 </worksheet>
 </file>
</xml_diff>